<commit_message>
Wykresy U_H dla alfa, B_n
</commit_message>
<xml_diff>
--- a/Spraw4/lab4.xlsx
+++ b/Spraw4/lab4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john\Documents\Janek\Uczelnia\Semestr3\Programy\FIZ31\Spraw4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john\Documents\Janek\Uczelnia\Semestr3\FIZ31\Spraw4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E34ECA5-4D1A-4E17-BB79-4F664AB167F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C83DE5-61E9-48B6-8309-0F039EEF2AC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Zamienie Indukcji B (kąt co 10 stopni)</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Przedzialka co 0.1 mA</t>
   </si>
   <si>
-    <t>56,49</t>
-  </si>
-  <si>
     <t>Kat:</t>
   </si>
   <si>
@@ -79,6 +76,15 @@
   </si>
   <si>
     <t>Drugie pomiary</t>
+  </si>
+  <si>
+    <t>ALPHA_0:</t>
+  </si>
+  <si>
+    <t>I[A]</t>
+  </si>
+  <si>
+    <t>U[V]</t>
   </si>
 </sst>
 </file>
@@ -193,6 +199,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>U_H</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>(B_n)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -224,19 +259,9 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.10954768153980753"/>
-          <c:y val="0.17171296296296298"/>
-          <c:w val="0.8668248031496063"/>
-          <c:h val="0.61498432487605714"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -245,10 +270,8 @@
             <c:v>U_H</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -268,244 +291,304 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
             <c:numRef>
-              <c:f>Arkusz1!$D$4:$D$39</c:f>
+              <c:f>Arkusz1!$K$4:$K$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-4.4349079341127418E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>-0.13011447762148057</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>-0.21193041063070422</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>-0.28731345613975895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>-0.35397545432421595</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>-0.409892962047336</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>-0.45336867199299496</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>-0.48308293234606114</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
+                  <c:v>-0.49813380320355832</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90</c:v>
+                  <c:v>-0.49806443385341675</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100</c:v>
+                  <c:v>-0.482876929917119</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>110</c:v>
+                  <c:v>-0.45303228943614393</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120</c:v>
+                  <c:v>-0.40943640984222751</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>130</c:v>
+                  <c:v>-0.35341259055268304</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>140</c:v>
+                  <c:v>-0.2866613658407508</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>150</c:v>
+                  <c:v>-0.21120888720489905</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>160</c:v>
+                  <c:v>-0.12934542202690102</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>170</c:v>
+                  <c:v>-4.3555835316440056E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>180</c:v>
+                  <c:v>4.3555835316440056E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>190</c:v>
+                  <c:v>0.12934542202690102</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>200</c:v>
+                  <c:v>0.21120888720489905</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>210</c:v>
+                  <c:v>0.2866613658407508</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>220</c:v>
+                  <c:v>0.35341259055268304</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>230</c:v>
+                  <c:v>0.40943640984222751</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>240</c:v>
+                  <c:v>0.45303228943614393</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>250</c:v>
+                  <c:v>0.482876929917119</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>260</c:v>
+                  <c:v>0.49806443385341675</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>270</c:v>
+                  <c:v>0.49813380320355832</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>280</c:v>
+                  <c:v>0.48308293234606114</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>290</c:v>
+                  <c:v>0.45336867199299496</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>300</c:v>
+                  <c:v>0.409892962047336</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>310</c:v>
+                  <c:v>0.35397545432421595</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>320</c:v>
+                  <c:v>0.28731345613975895</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>330</c:v>
+                  <c:v>0.21193041063070422</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>340</c:v>
+                  <c:v>0.13011447762148057</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>350</c:v>
+                  <c:v>4.4349079341127418E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Arkusz1!$G$4:$G$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>8.32</c:v>
+                  <c:v>8.320000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.8</c:v>
+                  <c:v>2.18E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.119999999999997</c:v>
+                  <c:v>3.4119999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46.42</c:v>
+                  <c:v>4.6420000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>56.49</c:v>
+                  <c:v>5.6489999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>64.67</c:v>
+                  <c:v>6.4670000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>71.510000000000005</c:v>
+                  <c:v>7.1510000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>75.95</c:v>
+                  <c:v>7.5950000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>78.23</c:v>
+                  <c:v>7.8230000000000008E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>78.209999999999994</c:v>
+                  <c:v>7.8209999999999988E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>75.709999999999994</c:v>
+                  <c:v>7.571E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>70.900000000000006</c:v>
+                  <c:v>7.0900000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>64.319999999999993</c:v>
+                  <c:v>6.4319999999999988E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>55.45</c:v>
+                  <c:v>5.5450000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>45.21</c:v>
+                  <c:v>4.521E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>33.75</c:v>
+                  <c:v>3.3750000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21.34</c:v>
+                  <c:v>2.1340000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.08</c:v>
+                  <c:v>8.0800000000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-5.05</c:v>
+                  <c:v>-5.0499999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-18.34</c:v>
+                  <c:v>-1.8339999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-30.73</c:v>
+                  <c:v>-3.073E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-41.9</c:v>
+                  <c:v>-4.19E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-51.61</c:v>
+                  <c:v>-5.1609999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-59.25</c:v>
+                  <c:v>-5.9249999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-65.42</c:v>
+                  <c:v>-6.5420000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-69.489999999999995</c:v>
+                  <c:v>-6.9489999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-71.790000000000006</c:v>
+                  <c:v>-7.1790000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-71.62</c:v>
+                  <c:v>-7.1620000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-69.66</c:v>
+                  <c:v>-6.966E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-65.17</c:v>
+                  <c:v>-6.5170000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-58.73</c:v>
+                  <c:v>-5.8729999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-50.44</c:v>
+                  <c:v>-5.0439999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-41.01</c:v>
+                  <c:v>-4.1009999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-29.71</c:v>
+                  <c:v>-2.971E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-17.14</c:v>
+                  <c:v>-1.7139999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-4.79</c:v>
+                  <c:v>-4.79E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000028-2FFD-446B-B60A-3A68C5B2EA57}"/>
+              <c16:uniqueId val="{00000000-9518-422D-8873-498BA023833E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -517,18 +600,86 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="1639144752"/>
-        <c:axId val="1646618192"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1639144752"/>
+        <c:axId val="655757391"/>
+        <c:axId val="642694703"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="655757391"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>B_n [T]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -538,8 +689,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -566,15 +717,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1646618192"/>
+        <c:crossAx val="642694703"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="1646618192"/>
+        <c:axId val="642694703"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -594,14 +742,84 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>U_H [V]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.1896486515165549E-2"/>
+              <c:y val="0.47964408090634914"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -625,9 +843,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1639144752"/>
+        <c:crossAx val="655757391"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -637,39 +855,8 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:dispBlanksAs val="gap"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -727,6 +914,42 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>U_H(</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="el-GR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>α</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -759,20 +982,18 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>U_H</c:v>
+            <c:v>U_H(alfa)</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -792,247 +1013,409 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
-              <c:f>Arkusz1!$K$3:$K$39</c:f>
+              <c:f>Arkusz1!$D$4:$D$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.27201055544468489</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.45647262536381383</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.49401581204643091</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.37255658023967442</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.13118742685196438</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.15240531055110834</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.38694534077894455</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.49694432696168761</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.44699833180027893</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.2531828205548794</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-2.2121339042535482E-2</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.29030559210615714</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.46505297509338089</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.49011982972015578</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.35743821481458232</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.10971262918950236</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.17332472774851515</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.40057631786691522</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.49889963934030013</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.43664864860699731</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.23385925917137948</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.4199356243765746E-2</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.30803210202668224</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.4727225774605584</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.48526400977090267</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.34161985190792538</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-8.8022973235605706E-2</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.19390471041461474</c:v>
+                  <c:v>280</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.41342281696104072</c:v>
+                  <c:v>290</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-0.49987791995057473</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.42544384432792981</c:v>
+                  <c:v>310</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-0.21407771404222578</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-6.6190814602725967E-2</c:v>
+                  <c:v>330</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.32515537008127626</c:v>
+                  <c:v>340</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-0.47946641252030658</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Arkusz1!$G$4:$G$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>8.32</c:v>
+                  <c:v>8.320000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.8</c:v>
+                  <c:v>2.18E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.119999999999997</c:v>
+                  <c:v>3.4119999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46.42</c:v>
+                  <c:v>4.6420000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>56.49</c:v>
+                  <c:v>5.6489999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>64.67</c:v>
+                  <c:v>6.4670000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>71.510000000000005</c:v>
+                  <c:v>7.1510000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>75.95</c:v>
+                  <c:v>7.5950000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>78.23</c:v>
+                  <c:v>7.8230000000000008E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>78.209999999999994</c:v>
+                  <c:v>7.8209999999999988E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>75.709999999999994</c:v>
+                  <c:v>7.571E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>70.900000000000006</c:v>
+                  <c:v>7.0900000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>64.319999999999993</c:v>
+                  <c:v>6.4319999999999988E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>55.45</c:v>
+                  <c:v>5.5450000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>45.21</c:v>
+                  <c:v>4.521E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>33.75</c:v>
+                  <c:v>3.3750000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21.34</c:v>
+                  <c:v>2.1340000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.08</c:v>
+                  <c:v>8.0800000000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-5.05</c:v>
+                  <c:v>-5.0499999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-18.34</c:v>
+                  <c:v>-1.8339999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-30.73</c:v>
+                  <c:v>-3.073E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-41.9</c:v>
+                  <c:v>-4.19E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-51.61</c:v>
+                  <c:v>-5.1609999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-59.25</c:v>
+                  <c:v>-5.9249999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-65.42</c:v>
+                  <c:v>-6.5420000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-69.489999999999995</c:v>
+                  <c:v>-6.9489999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-71.790000000000006</c:v>
+                  <c:v>-7.1790000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-71.62</c:v>
+                  <c:v>-7.1620000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-69.66</c:v>
+                  <c:v>-6.966E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-65.17</c:v>
+                  <c:v>-6.5170000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-58.73</c:v>
+                  <c:v>-5.8729999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-50.44</c:v>
+                  <c:v>-5.0439999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-41.01</c:v>
+                  <c:v>-4.1009999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-29.71</c:v>
+                  <c:v>-2.971E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-17.14</c:v>
+                  <c:v>-1.7139999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-4.79</c:v>
+                  <c:v>-4.79E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-0D4C-499E-BC70-3A3DE12B9DAA}"/>
+              <c16:uniqueId val="{00000000-46C5-47F6-9B66-F94B1AA6632D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>S_alfa</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="5"/>
+            <c:backward val="5"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$D$19:$D$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$G$19:$G$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3.3750000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1340000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0800000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5.0499999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.8339999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3.073E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4.19E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-5.1609999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.9249999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-6.5420000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-6.9489999999999996E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-46C5-47F6-9B66-F94B1AA6632D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1044,18 +1427,96 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="1850513584"/>
-        <c:axId val="1646634416"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1850513584"/>
+        <c:axId val="643010479"/>
+        <c:axId val="594533551"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="643010479"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="el-GR">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>α</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t> [˚]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1065,8 +1526,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1093,15 +1554,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1646634416"/>
+        <c:crossAx val="594533551"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="1646634416"/>
+        <c:axId val="594533551"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1121,14 +1579,76 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>U_H [V]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1152,9 +1672,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1850513584"/>
+        <c:crossAx val="643010479"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1164,8 +1684,65 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1179,7 +1756,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1194,16 +1771,461 @@
           <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
-    </c:legend>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$G$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>U[V]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="5.000000000000001E-3"/>
+            <c:backward val="5.000000000000001E-3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$F$46:$F$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.9999999999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$G$46:$G$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>8.320000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.093E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.273E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.456E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6289999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7950000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9649999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1309999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3050000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4920000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.605E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B926-47FB-ACD7-AD069AF5ABFF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="697728223"/>
+        <c:axId val="594543535"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="697728223"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>I</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> [A]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="594543535"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="594543535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>U_H [V]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="697728223"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1319,8 +2341,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1347,8 +2409,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1449,7 +2511,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1481,10 +2543,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1524,22 +2586,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1644,8 +2707,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1777,19 +2840,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1803,6 +2867,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1823,7 +2898,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1850,8 +2925,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1952,7 +3027,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1984,10 +3059,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2027,22 +3102,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2147,8 +3223,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2280,19 +3356,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2306,6 +3383,533 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2330,22 +3934,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>404309</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>123937</xdr:rowOff>
+      <xdr:colOff>367144</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>138545</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>510989</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>41563</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>41562</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Wykres 1">
+        <xdr:cNvPr id="4" name="Wykres 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98CE44B7-20D4-430A-8D57-AF419933980E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DA2CDEF-4F42-43A0-9413-31CACA42CF4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2366,22 +3970,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>327211</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>116539</xdr:rowOff>
+      <xdr:colOff>337456</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>97971</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>44823</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>161364</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>43542</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Wykres 2">
+        <xdr:cNvPr id="5" name="Wykres 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0D42FEE-FC49-406D-881C-371508D596D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45C994B4-9D4D-4AEA-94FD-851C9B8D0FE5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2394,6 +3998,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>10885</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>32657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>478971</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>130627</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Wykres 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{373806FC-358E-4A26-88B2-DA5E18EDC606}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2665,10 +4305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K810"/>
+  <dimension ref="B1:AA810"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2681,12 +4321,15 @@
     <col min="11" max="11" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:27" x14ac:dyDescent="0.3">
       <c r="I1"/>
       <c r="J1"/>
       <c r="K1"/>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="AA1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2703,16 +4346,22 @@
         <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>8.32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2720,13 +4369,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>2</v>
@@ -2740,12 +4389,14 @@
       <c r="J3" s="2">
         <v>0.05</v>
       </c>
-      <c r="K3" s="2">
-        <f>$I$3*SIN(D4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <v>175</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1">
         <v>1</v>
@@ -2760,18 +4411,22 @@
         <v>8</v>
       </c>
       <c r="G4" s="1">
-        <v>8.32</v>
+        <f>AA2/1000</f>
+        <v>8.320000000000001E-3</v>
       </c>
       <c r="H4" s="1"/>
       <c r="J4" s="2">
         <v>0.05</v>
       </c>
       <c r="K4" s="2">
-        <f>$I$3*SIN(D5)</f>
-        <v>-0.27201055544468489</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+        <f>$I$3*SIN((D4-$L$3)*(3.14/180))</f>
+        <v>-4.4349079341127418E-2</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>34.119999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1">
         <v>2</v>
@@ -2784,18 +4439,22 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1">
-        <v>21.8</v>
+        <f t="shared" ref="G5:G39" si="0">AA3/1000</f>
+        <v>2.18E-2</v>
       </c>
       <c r="H5" s="1"/>
       <c r="J5" s="2">
         <v>0.05</v>
       </c>
       <c r="K5" s="2">
-        <f>$I$3*SIN(D6)</f>
-        <v>0.45647262536381383</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" ref="K5:K39" si="1">$I$3*SIN((D5-$L$3)*(3.14/180))</f>
+        <v>-0.13011447762148057</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>46.42</v>
+      </c>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="1">
         <v>3</v>
@@ -2808,18 +4467,22 @@
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1">
-        <v>34.119999999999997</v>
+        <f t="shared" si="0"/>
+        <v>3.4119999999999998E-2</v>
       </c>
       <c r="H6" s="1"/>
       <c r="J6" s="2">
         <v>0.05</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" ref="K6:K39" si="0">$I$3*SIN(D7)</f>
-        <v>-0.49401581204643091</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.21193041063070422</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>56.49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1">
         <v>4</v>
@@ -2832,18 +4495,22 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1">
-        <v>46.42</v>
+        <f t="shared" si="0"/>
+        <v>4.6420000000000003E-2</v>
       </c>
       <c r="H7" s="1"/>
       <c r="J7" s="2">
         <v>0.05</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="0"/>
-        <v>0.37255658023967442</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.28731345613975895</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>64.67</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1">
         <v>5</v>
@@ -2856,18 +4523,22 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1">
-        <v>56.49</v>
+        <f t="shared" si="0"/>
+        <v>5.6489999999999999E-2</v>
       </c>
       <c r="H8" s="1"/>
       <c r="J8" s="2">
         <v>0.05</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.13118742685196438</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.35397545432421595</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>71.510000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1">
         <v>6</v>
@@ -2880,18 +4551,22 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1">
-        <v>64.67</v>
+        <f t="shared" si="0"/>
+        <v>6.4670000000000005E-2</v>
       </c>
       <c r="H9" s="1"/>
       <c r="J9" s="2">
         <v>0.05</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.15240531055110834</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.409892962047336</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>75.95</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1">
         <v>7</v>
@@ -2904,18 +4579,22 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1">
-        <v>71.510000000000005</v>
+        <f t="shared" si="0"/>
+        <v>7.1510000000000004E-2</v>
       </c>
       <c r="H10" s="1"/>
       <c r="J10" s="2">
         <v>0.05</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" si="0"/>
-        <v>0.38694534077894455</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.45336867199299496</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>78.23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1">
         <v>8</v>
@@ -2928,18 +4607,22 @@
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1">
-        <v>75.95</v>
+        <f t="shared" si="0"/>
+        <v>7.5950000000000004E-2</v>
       </c>
       <c r="H11" s="1"/>
       <c r="J11" s="2">
         <v>0.05</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.49694432696168761</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.48308293234606114</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>78.209999999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1">
         <v>9</v>
@@ -2952,18 +4635,22 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1">
-        <v>78.23</v>
+        <f t="shared" si="0"/>
+        <v>7.8230000000000008E-2</v>
       </c>
       <c r="H12" s="1"/>
       <c r="J12" s="2">
         <v>0.05</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" si="0"/>
-        <v>0.44699833180027893</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.49813380320355832</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>75.709999999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1">
         <v>10</v>
@@ -2976,18 +4663,22 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1">
-        <v>78.209999999999994</v>
+        <f t="shared" si="0"/>
+        <v>7.8209999999999988E-2</v>
       </c>
       <c r="H13" s="1"/>
       <c r="J13" s="2">
         <v>0.05</v>
       </c>
       <c r="K13" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.2531828205548794</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.49806443385341675</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>70.900000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1">
         <v>11</v>
@@ -3000,18 +4691,22 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1">
-        <v>75.709999999999994</v>
+        <f t="shared" si="0"/>
+        <v>7.571E-2</v>
       </c>
       <c r="H14" s="1"/>
       <c r="J14" s="2">
         <v>0.05</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="0"/>
-        <v>-2.2121339042535482E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.482876929917119</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>64.319999999999993</v>
+      </c>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1">
         <v>12</v>
@@ -3024,18 +4719,22 @@
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1">
-        <v>70.900000000000006</v>
+        <f t="shared" si="0"/>
+        <v>7.0900000000000005E-2</v>
       </c>
       <c r="H15" s="1"/>
       <c r="J15" s="2">
         <v>0.05</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="0"/>
-        <v>0.29030559210615714</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.45303228943614393</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>55.45</v>
+      </c>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1">
         <v>13</v>
@@ -3048,18 +4747,22 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1">
-        <v>64.319999999999993</v>
+        <f t="shared" si="0"/>
+        <v>6.4319999999999988E-2</v>
       </c>
       <c r="H16" s="1"/>
       <c r="J16" s="2">
         <v>0.05</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.46505297509338089</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.40943640984222751</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>45.21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1">
         <v>14</v>
@@ -3072,18 +4775,22 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1">
-        <v>55.45</v>
+        <f t="shared" si="0"/>
+        <v>5.5450000000000006E-2</v>
       </c>
       <c r="H17" s="1"/>
       <c r="J17" s="2">
         <v>0.05</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" si="0"/>
-        <v>0.49011982972015578</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.35341259055268304</v>
+      </c>
+      <c r="AA17" s="1">
+        <v>33.75</v>
+      </c>
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1">
         <v>15</v>
@@ -3096,18 +4803,22 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1">
-        <v>45.21</v>
+        <f t="shared" si="0"/>
+        <v>4.521E-2</v>
       </c>
       <c r="H18" s="1"/>
       <c r="J18" s="2">
         <v>0.05</v>
       </c>
       <c r="K18" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.35743821481458232</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.2866613658407508</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>21.34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1">
         <v>16</v>
@@ -3120,18 +4831,22 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1">
-        <v>33.75</v>
+        <f t="shared" si="0"/>
+        <v>3.3750000000000002E-2</v>
       </c>
       <c r="H19" s="1"/>
       <c r="J19" s="2">
         <v>0.05</v>
       </c>
       <c r="K19" s="2">
-        <f t="shared" si="0"/>
-        <v>0.10971262918950236</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.21120888720489905</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>8.08</v>
+      </c>
+    </row>
+    <row r="20" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1">
         <v>17</v>
@@ -3144,18 +4859,22 @@
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1">
-        <v>21.34</v>
+        <f t="shared" si="0"/>
+        <v>2.1340000000000001E-2</v>
       </c>
       <c r="H20" s="1"/>
       <c r="J20" s="2">
         <v>0.05</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17332472774851515</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.12934542202690102</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>-5.05</v>
+      </c>
+    </row>
+    <row r="21" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1">
         <v>18</v>
@@ -3168,18 +4887,22 @@
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1">
-        <v>8.08</v>
+        <f t="shared" si="0"/>
+        <v>8.0800000000000004E-3</v>
       </c>
       <c r="H21" s="1"/>
       <c r="J21" s="2">
         <v>0.05</v>
       </c>
       <c r="K21" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.40057631786691522</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-4.3555835316440056E-2</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>-18.34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1">
         <v>19</v>
@@ -3192,18 +4915,22 @@
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1">
-        <v>-5.05</v>
+        <f t="shared" si="0"/>
+        <v>-5.0499999999999998E-3</v>
       </c>
       <c r="H22" s="1"/>
       <c r="J22" s="2">
         <v>0.05</v>
       </c>
       <c r="K22" s="2">
-        <f t="shared" si="0"/>
-        <v>0.49889963934030013</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>4.3555835316440056E-2</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>-30.73</v>
+      </c>
+    </row>
+    <row r="23" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1">
         <v>20</v>
@@ -3216,18 +4943,22 @@
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1">
-        <v>-18.34</v>
+        <f t="shared" si="0"/>
+        <v>-1.8339999999999999E-2</v>
       </c>
       <c r="H23" s="1"/>
       <c r="J23" s="2">
         <v>0.05</v>
       </c>
       <c r="K23" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.43664864860699731</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.12934542202690102</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>-41.9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1">
         <v>21</v>
@@ -3240,18 +4971,22 @@
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1">
-        <v>-30.73</v>
+        <f t="shared" si="0"/>
+        <v>-3.073E-2</v>
       </c>
       <c r="H24" s="1"/>
       <c r="J24" s="2">
         <v>0.05</v>
       </c>
       <c r="K24" s="2">
-        <f t="shared" si="0"/>
-        <v>0.23385925917137948</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.21120888720489905</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>-51.61</v>
+      </c>
+    </row>
+    <row r="25" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1">
         <v>22</v>
@@ -3264,18 +4999,22 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1">
-        <v>-41.9</v>
+        <f t="shared" si="0"/>
+        <v>-4.19E-2</v>
       </c>
       <c r="H25" s="1"/>
       <c r="J25" s="2">
         <v>0.05</v>
       </c>
       <c r="K25" s="2">
-        <f t="shared" si="0"/>
-        <v>4.4199356243765746E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.2866613658407508</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>-59.25</v>
+      </c>
+    </row>
+    <row r="26" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="1">
         <v>23</v>
@@ -3288,18 +5027,22 @@
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1">
-        <v>-51.61</v>
+        <f t="shared" si="0"/>
+        <v>-5.1609999999999996E-2</v>
       </c>
       <c r="H26" s="1"/>
       <c r="J26" s="2">
         <v>0.05</v>
       </c>
       <c r="K26" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.30803210202668224</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.35341259055268304</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>-65.42</v>
+      </c>
+    </row>
+    <row r="27" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="1">
         <v>24</v>
@@ -3312,18 +5055,22 @@
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1">
-        <v>-59.25</v>
+        <f t="shared" si="0"/>
+        <v>-5.9249999999999997E-2</v>
       </c>
       <c r="H27" s="1"/>
       <c r="J27" s="2">
         <v>0.05</v>
       </c>
       <c r="K27" s="2">
-        <f t="shared" si="0"/>
-        <v>0.4727225774605584</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.40943640984222751</v>
+      </c>
+      <c r="AA27" s="1">
+        <v>-69.489999999999995</v>
+      </c>
+    </row>
+    <row r="28" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="1">
         <v>25</v>
@@ -3336,18 +5083,22 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1">
-        <v>-65.42</v>
+        <f t="shared" si="0"/>
+        <v>-6.5420000000000006E-2</v>
       </c>
       <c r="H28" s="1"/>
       <c r="J28" s="2">
         <v>0.05</v>
       </c>
       <c r="K28" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.48526400977090267</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.45303228943614393</v>
+      </c>
+      <c r="AA28" s="1">
+        <v>-71.790000000000006</v>
+      </c>
+    </row>
+    <row r="29" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="C29" s="1">
         <v>26</v>
@@ -3360,18 +5111,22 @@
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1">
-        <v>-69.489999999999995</v>
+        <f t="shared" si="0"/>
+        <v>-6.9489999999999996E-2</v>
       </c>
       <c r="H29" s="1"/>
       <c r="J29" s="2">
         <v>0.05</v>
       </c>
       <c r="K29" s="2">
-        <f t="shared" si="0"/>
-        <v>0.34161985190792538</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.482876929917119</v>
+      </c>
+      <c r="AA29" s="1">
+        <v>-71.62</v>
+      </c>
+    </row>
+    <row r="30" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="1">
         <v>27</v>
@@ -3384,18 +5139,22 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1">
-        <v>-71.790000000000006</v>
+        <f t="shared" si="0"/>
+        <v>-7.1790000000000007E-2</v>
       </c>
       <c r="H30" s="1"/>
       <c r="J30" s="2">
         <v>0.05</v>
       </c>
       <c r="K30" s="2">
-        <f t="shared" si="0"/>
-        <v>-8.8022973235605706E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.49806443385341675</v>
+      </c>
+      <c r="AA30" s="1">
+        <v>-69.66</v>
+      </c>
+    </row>
+    <row r="31" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="C31" s="1">
         <v>28</v>
@@ -3408,18 +5167,22 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1">
-        <v>-71.62</v>
+        <f t="shared" si="0"/>
+        <v>-7.1620000000000003E-2</v>
       </c>
       <c r="H31" s="1"/>
       <c r="J31" s="2">
         <v>0.05</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.19390471041461474</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.49813380320355832</v>
+      </c>
+      <c r="AA31" s="1">
+        <v>-65.17</v>
+      </c>
+    </row>
+    <row r="32" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="C32" s="1">
         <v>29</v>
@@ -3432,18 +5195,22 @@
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1">
-        <v>-69.66</v>
+        <f t="shared" si="0"/>
+        <v>-6.966E-2</v>
       </c>
       <c r="H32" s="1"/>
       <c r="J32" s="2">
         <v>0.05</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" si="0"/>
-        <v>0.41342281696104072</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.48308293234606114</v>
+      </c>
+      <c r="AA32" s="1">
+        <v>-58.73</v>
+      </c>
+    </row>
+    <row r="33" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="1">
         <v>30</v>
@@ -3456,18 +5223,22 @@
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1">
-        <v>-65.17</v>
+        <f t="shared" si="0"/>
+        <v>-6.5170000000000006E-2</v>
       </c>
       <c r="H33" s="1"/>
       <c r="J33" s="2">
         <v>0.05</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.49987791995057473</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.45336867199299496</v>
+      </c>
+      <c r="AA33" s="1">
+        <v>-50.44</v>
+      </c>
+    </row>
+    <row r="34" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="C34" s="1">
         <v>31</v>
@@ -3480,18 +5251,22 @@
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1">
-        <v>-58.73</v>
+        <f t="shared" si="0"/>
+        <v>-5.8729999999999997E-2</v>
       </c>
       <c r="H34" s="1"/>
       <c r="J34" s="2">
         <v>0.05</v>
       </c>
       <c r="K34" s="2">
-        <f t="shared" si="0"/>
-        <v>0.42544384432792981</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.409892962047336</v>
+      </c>
+      <c r="AA34" s="1">
+        <v>-41.01</v>
+      </c>
+    </row>
+    <row r="35" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="C35" s="1">
         <v>32</v>
@@ -3504,18 +5279,22 @@
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1">
-        <v>-50.44</v>
+        <f t="shared" si="0"/>
+        <v>-5.0439999999999999E-2</v>
       </c>
       <c r="H35" s="1"/>
       <c r="J35" s="2">
         <v>0.05</v>
       </c>
       <c r="K35" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.21407771404222578</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.35397545432421595</v>
+      </c>
+      <c r="AA35" s="1">
+        <v>-29.71</v>
+      </c>
+    </row>
+    <row r="36" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="C36" s="1">
         <v>33</v>
@@ -3528,18 +5307,22 @@
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1">
-        <v>-41.01</v>
+        <f t="shared" si="0"/>
+        <v>-4.1009999999999998E-2</v>
       </c>
       <c r="H36" s="1"/>
       <c r="J36" s="2">
         <v>0.05</v>
       </c>
       <c r="K36" s="2">
-        <f t="shared" si="0"/>
-        <v>-6.6190814602725967E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.28731345613975895</v>
+      </c>
+      <c r="AA36" s="1">
+        <v>-17.14</v>
+      </c>
+    </row>
+    <row r="37" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
       <c r="C37" s="1">
         <v>34</v>
@@ -3552,18 +5335,22 @@
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1">
-        <v>-29.71</v>
+        <f t="shared" si="0"/>
+        <v>-2.971E-2</v>
       </c>
       <c r="H37" s="1"/>
       <c r="J37" s="2">
         <v>0.05</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="0"/>
-        <v>0.32515537008127626</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.21193041063070422</v>
+      </c>
+      <c r="AA37" s="1">
+        <v>-4.79</v>
+      </c>
+    </row>
+    <row r="38" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="1">
         <v>35</v>
@@ -3576,18 +5363,19 @@
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1">
-        <v>-17.14</v>
+        <f t="shared" si="0"/>
+        <v>-1.7139999999999999E-2</v>
       </c>
       <c r="H38" s="1"/>
       <c r="J38" s="2">
         <v>0.05</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" si="0"/>
-        <v>-0.47946641252030658</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.13011447762148057</v>
+      </c>
+    </row>
+    <row r="39" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="C39" s="1">
         <v>36</v>
@@ -3600,91 +5388,121 @@
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1">
-        <v>-4.79</v>
+        <f t="shared" si="0"/>
+        <v>-4.79E-3</v>
       </c>
       <c r="H39" s="1"/>
       <c r="J39" s="2">
         <v>0.05</v>
       </c>
       <c r="K39" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>4.4349079341127418E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:27" x14ac:dyDescent="0.3">
       <c r="I40"/>
       <c r="J40"/>
-      <c r="K40"/>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="2:27" x14ac:dyDescent="0.3">
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="I41"/>
       <c r="J41"/>
       <c r="K41"/>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:27" x14ac:dyDescent="0.3">
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="I42"/>
       <c r="J42"/>
       <c r="K42"/>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:27" x14ac:dyDescent="0.3">
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="I43"/>
       <c r="J43"/>
       <c r="K43"/>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:27" x14ac:dyDescent="0.3">
       <c r="C44" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D44" s="3"/>
       <c r="I44"/>
       <c r="J44"/>
       <c r="K44"/>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:27" x14ac:dyDescent="0.3">
       <c r="C45" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>2</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="I45"/>
       <c r="J45"/>
       <c r="K45"/>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:27" x14ac:dyDescent="0.3">
       <c r="C46" s="3">
         <v>5</v>
       </c>
       <c r="D46" s="3">
         <v>8.32</v>
+      </c>
+      <c r="F46" s="3">
+        <f>C46/1000</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G46" s="3">
+        <f>D46/1000</f>
+        <v>8.320000000000001E-3</v>
       </c>
       <c r="I46"/>
       <c r="J46"/>
       <c r="K46"/>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:27" x14ac:dyDescent="0.3">
       <c r="C47" s="3">
         <v>6</v>
       </c>
       <c r="D47" s="3">
         <v>10.93</v>
+      </c>
+      <c r="F47" s="3">
+        <f t="shared" ref="F47:F56" si="2">C47/1000</f>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G47" s="3">
+        <f t="shared" ref="G47:G56" si="3">D47/1000</f>
+        <v>1.093E-2</v>
       </c>
       <c r="I47"/>
       <c r="J47"/>
       <c r="K47"/>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:27" x14ac:dyDescent="0.3">
       <c r="C48" s="3">
         <v>7</v>
       </c>
       <c r="D48" s="3">
         <v>12.73</v>
+      </c>
+      <c r="F48" s="3">
+        <f t="shared" si="2"/>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G48" s="3">
+        <f t="shared" si="3"/>
+        <v>1.273E-2</v>
       </c>
       <c r="I48"/>
       <c r="J48"/>
@@ -3697,6 +5515,14 @@
       <c r="D49" s="3">
         <v>14.56</v>
       </c>
+      <c r="F49" s="3">
+        <f t="shared" si="2"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G49" s="3">
+        <f t="shared" si="3"/>
+        <v>1.456E-2</v>
+      </c>
       <c r="I49"/>
       <c r="J49"/>
       <c r="K49"/>
@@ -3708,6 +5534,14 @@
       <c r="D50" s="3">
         <v>16.29</v>
       </c>
+      <c r="F50" s="3">
+        <f t="shared" si="2"/>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G50" s="3">
+        <f t="shared" si="3"/>
+        <v>1.6289999999999999E-2</v>
+      </c>
       <c r="I50"/>
       <c r="J50"/>
       <c r="K50"/>
@@ -3719,6 +5553,14 @@
       <c r="D51" s="3">
         <v>17.95</v>
       </c>
+      <c r="F51" s="3">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="G51" s="3">
+        <f t="shared" si="3"/>
+        <v>1.7950000000000001E-2</v>
+      </c>
       <c r="I51"/>
       <c r="J51"/>
       <c r="K51"/>
@@ -3730,6 +5572,14 @@
       <c r="D52" s="3">
         <v>19.649999999999999</v>
       </c>
+      <c r="F52" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G52" s="3">
+        <f t="shared" si="3"/>
+        <v>1.9649999999999997E-2</v>
+      </c>
       <c r="I52"/>
       <c r="J52"/>
       <c r="K52"/>
@@ -3741,6 +5591,14 @@
       <c r="D53" s="3">
         <v>21.31</v>
       </c>
+      <c r="F53" s="3">
+        <f t="shared" si="2"/>
+        <v>1.2E-2</v>
+      </c>
+      <c r="G53" s="3">
+        <f t="shared" si="3"/>
+        <v>2.1309999999999999E-2</v>
+      </c>
       <c r="I53"/>
       <c r="J53"/>
       <c r="K53"/>
@@ -3752,6 +5610,14 @@
       <c r="D54" s="3">
         <v>23.05</v>
       </c>
+      <c r="F54" s="3">
+        <f t="shared" si="2"/>
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="G54" s="3">
+        <f t="shared" si="3"/>
+        <v>2.3050000000000001E-2</v>
+      </c>
       <c r="I54"/>
       <c r="J54"/>
       <c r="K54"/>
@@ -3763,6 +5629,14 @@
       <c r="D55" s="3">
         <v>24.92</v>
       </c>
+      <c r="F55" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4E-2</v>
+      </c>
+      <c r="G55" s="3">
+        <f t="shared" si="3"/>
+        <v>2.4920000000000001E-2</v>
+      </c>
       <c r="I55"/>
       <c r="J55"/>
       <c r="K55"/>
@@ -3773,6 +5647,14 @@
       </c>
       <c r="D56" s="3">
         <v>26.05</v>
+      </c>
+      <c r="F56" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G56" s="3">
+        <f t="shared" si="3"/>
+        <v>2.605E-2</v>
       </c>
       <c r="I56"/>
       <c r="J56"/>
@@ -7549,6 +9431,9 @@
       <c r="K810"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K47:K82">
+    <sortCondition ref="K47"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>